<commit_message>
update filename, update html
</commit_message>
<xml_diff>
--- a/assets/Images/Data.xlsx
+++ b/assets/Images/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hacktiv8\Group Project 1 - Website eCommerce\Assets\Images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hacktiv8\Group Project 1 - Website eCommerce\hacktivate_fashion_store\Assets\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BAFD82-4AA8-44F4-922A-F527E4354D1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73167793-2F4F-4FF7-8F93-572369628ED8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C87C6F5C-A817-4C6F-89FA-6AFB4F8111DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -79,6 +79,123 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>BAHAN KATUN STRETCH
+MODEL SLIM FIT
+KANTONG HIDUP
+SIZE CHAT :
+LINGKAR DADA X PANJANG BAJU
+- XS : 88CM X 65CM
+- S : 90CM X 65CM
+- M : 100CM X 70CM
+- L : 102CM X 70CM
+- XL : 104CM X 71CM</t>
+  </si>
+  <si>
+    <t>Kaos : MARCELO BURLON
+Warna: Black,White
+Barang Kualitas IMPORT</t>
+  </si>
+  <si>
+    <t>Celana jeans berbahan Twill sangat nyaman di pakai karena bisa menyesuaian dengan bentuk kaki.
+Bahan denim di percaya tidak kaku sehingga kenyamanan saat memakainya lebih optimal
+Tersedia ukuran 28303234
+Size Chart
+28 : Waist 76 CM | Length 95 CM
+30 : Waist 80 CM | Length 96 CM
+32 : Waist 86 CM | Length 97 CM
+34 : Waist 90 CM | Length 98 CM</t>
+  </si>
+  <si>
+    <t>SEAL Celana Jogger Terbaru dari Okechuku
+Warna :
+1. Hijau TNI lembut
+2. Abu Tua
+3. Abu muda terang mendekati putih
+4. Hitam
+Bahan : Baby Terry
+Bahan baby terry berkualitas dengan halus, tidak panas dan nyaman di gunakan. Cocok untuk di pakai segala macam aktifitas, baik untuk hangout, nongkrong bareng teman, mau pun untuk olah raga.</t>
+  </si>
+  <si>
+    <t>FRANS Celana Jogger Pria Okechuku
+Celana Jogger yang sedang jadi Trenmodel sekarang ini dengan model Simple Basic sekaligus Elegan dilengkapi dengan variasi kecil di bagian kantong samping, juga kantong belakang. Terdapat tali di bagian depan.
+Cocok di padupadankan dengan berbagai tipe atasan.
+Cocok dipakai sehari-hari, buat nongkrong bareng teman, maupun untuk nge gym/olah raga.
+Material : Baby Terry (berkualitas, tekstur lembut, nyaman dipakai).
+Pilihan warna :
+1. Hitam
+2. Navy
+3. Abu tua
+4. Abu muda
+AllSize Fit to L
+Lingkar pinggang: 70 fit to 88 cm
+Panjang celana: 94 cm</t>
+  </si>
+  <si>
+    <t>Warna : Army
+Bahan : Twill (BAHAN TIDAK STRETCH)
+Detail : Bahan berkualitas dengan tekstur halus dan nyaman di gunakan. Cocok untuk di pakai segala macam aktifitas, baik untuk hangout, nongkrong bareng teman, mau pun untuk olah raga.
+Terdapat kantong di kiri dan kanan, juga di kanan belakang. Terdapat tali di bagian pinggang depan.
+*M/L (M fit to L)*
+Lingkar pinggang : 72cm fit to 84cm
+Panjang celana: 94cm
+Lingkar pinggul 116cm
+Lingkar paha 64cm
+*XL/XXL (XL fit to XXL)*
+Lingkar pinggang : 74cm fit to 88cm
+Panjang celana : 94cm
+Lingkar pinggul 120cm
+Lingkar paha 66cm</t>
+  </si>
+  <si>
+    <t>FITUR PRODUK
+1. Canvas Series
+2. 6 slot untuk menyimpan kartu
+3. 2 slot kantung sisip tersembunyi
+4. 2 ruang utama untuk menyimpan uang
+.
+Dimensi : 23 x 9 x 1 cm (Keadaan terbuka)
+Ukuran : Horizontal
+Warna : Black, Brown, Grey, Blue, Maroon &amp; Green
+Material : Canvas Leather</t>
+  </si>
+  <si>
+    <t>FITUR PRODUK
+1. Canvas Series
+2. 6 slot untuk menyimpan kartu
+3. 2 slot kantung sisip tersembunyi
+4. 2 ruang utama untuk menyimpan uang
+.
+Dimensi : 19 x 12 x 1 cm (Keadaan Terbuka)
+Ukuran : Vertical
+Warna : Black, Brown, Grey, Blue, Green, Maroon &amp; Apricot
+Material : Canvas Leather
+Fungsi : Menyimpan Barang Berharga Seperti Uang, Kartu Identitas, Debit/Credit Card, Photo, Dll.
+.</t>
+  </si>
+  <si>
+    <t>FITUR PRODUK
+1. Canvas Series
+2. 10 slot untuk menyimpan kartu
+3. 2 slot kantung sisip tersembunyi
+4. 2 ruang utama untuk menyimpan uang
+5. 1 slot untuk menyimpan foto atau kartu tanda pengenal
+.
+Dimensi : 18 x 17,5 x 1 cm
+Ukuran : Long
+Warna : Black, Brown, Grey, Blue, Green, Maroon &amp; Apricot
+Material : Canvas Leather</t>
+  </si>
+  <si>
+    <t>Dompet pendek/lipat
+Warna : Hitam : HABIS
+Coklat
+Ukuran : 10 x 1.5 x 12 cm
+Bahan : Kulit pu</t>
   </si>
 </sst>
 </file>
@@ -97,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +224,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -138,6 +261,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -454,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61848B43-4CA2-4F81-BADC-1A257811EF8F}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,10 +591,12 @@
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="25.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="57.88671875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="8.88671875" style="6"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,8 +609,11 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -493,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -505,7 +636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A18" si="0">A3+1</f>
         <v>3</v>
@@ -516,8 +647,11 @@
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -531,8 +665,11 @@
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>A5+1</f>
         <v>5</v>
@@ -543,8 +680,11 @@
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G7" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -555,8 +695,11 @@
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G8" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -570,8 +713,11 @@
       <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G9" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f>A9+1</f>
         <v>8</v>
@@ -582,8 +728,11 @@
       <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f>A10+1</f>
         <v>9</v>
@@ -594,8 +743,11 @@
       <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -606,8 +758,11 @@
       <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -621,8 +776,11 @@
       <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -633,8 +791,11 @@
       <c r="D15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G15" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>13</v>

</xml_diff>